<commit_message>
Performance Opts, Update Todos, more inlines
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>PBI</t>
   </si>
@@ -53,19 +53,10 @@
     <t>Render the terrain</t>
   </si>
   <si>
-    <t>Mouse-ray-heightmap intersection testing</t>
-  </si>
-  <si>
     <t>Paint Blend-texture where the intersection is</t>
   </si>
   <si>
     <t>OnMouseDown: Modify terrain heightmap based on blend texture</t>
-  </si>
-  <si>
-    <t>Allow importing of 3ds models</t>
-  </si>
-  <si>
-    <t>Allow creation of objects: {Box, Sphere}</t>
   </si>
   <si>
     <t>Basic Lighting</t>
@@ -114,9 +105,6 @@
     <t>Make sure things like Fresnel base color parameters are in SMaterialLayer</t>
   </si>
   <si>
-    <t>Add SMaterialLayer containg all maps and a blend mask</t>
-  </si>
-  <si>
     <t>Add Imaterial, a collection of (at maximum 8) SMaterialLayers</t>
   </si>
   <si>
@@ -199,13 +187,61 @@
   </si>
   <si>
     <t>Support Alpha blending, alpha taken from Diff tex, if bAlphaBlend enabled in material</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add SMaterialLayer containg all maps and a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>blend mask</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Implement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mouse-ray-heightmap intersection testing</t>
+    </r>
+  </si>
+  <si>
+    <t>Draw rubberband</t>
+  </si>
+  <si>
+    <t>Allow importing of 3ds models, use Engine's 3DS File loader</t>
+  </si>
+  <si>
+    <t>Allow creation of primitive objects: {Box, Sphere}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +260,13 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-9.9978637043366805E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -333,6 +376,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -618,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,22 +687,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>30</v>
+      <c r="B3" s="19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -675,235 +719,240 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="B8" s="18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="16" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
+    <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
-      <c r="B25" s="6" t="s">
-        <v>25</v>
+      <c r="B25" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>21</v>
+      <c r="A26" s="15"/>
+      <c r="B26" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B34" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="6" t="s">
+    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="B43" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use Vec3, Fixes for RayHeightInt, Fixes for stage data sampling
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>PBI</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Allow creation of primitive objects: {Box, Sphere}</t>
+  </si>
+  <si>
+    <t>[ENGINE] Object::Hide() function</t>
   </si>
 </sst>
 </file>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,210 +751,215 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+    <row r="16" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+    <row r="17" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="20" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="3" t="s">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    <row r="22" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="8" t="s">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="7" t="s">
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+    <row r="31" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+    <row r="34" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+    <row r="35" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="6" t="s">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
+      <c r="B38" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+    <row r="39" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="8" t="s">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    <row r="41" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="6" t="s">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>